<commit_message>
First test for User Part. If programmers have any problems to understand my feedback, please write on the "programmer check" on the test excel, OR you can chat with me online in the group.
</commit_message>
<xml_diff>
--- a/test/Test.xlsx
+++ b/test/Test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigbigcyan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/DUS/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AEA571F-25DE-6048-9877-A2973725EE21}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFF1477-8C78-4145-A278-03C5B84572D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{2CF56C27-F1AE-2F4B-AFC0-F9C85D1AAA72}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -312,12 +312,71 @@
 1) has been completed, 
 can test 1) first</t>
   </si>
+  <si>
+    <t>S2
+1. email address should be unique, but I used same email to register, register function could work. That's not right.
+2. when I input an inlegal email address, the box border will be red(that's right), but I suggest that it should show some reminder(shown on the page or some alert box) to remind user to input a valid email. That will be better.
+3. I have not recieved any confirmation code when I register(I know it has not completed, I just mention it)
+4.the password should be inputted twice for double check.
+5.the password should be 6-20 length.
+6.the password should only contain letters and numbers, but when I input  this:"," it also could work.
+7.just suggestion on the page:
+7.1 "ID", this word, may make confuse to users, it can be changed to "username"
+7.2 "name" may be divided into "first name" and "last name". That will be better I think.</t>
+  </si>
+  <si>
+    <t>it has not completed, right?</t>
+  </si>
+  <si>
+    <t>well done
+I think when the register part is completed, the login part is fine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+well done
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">S2
+1. no confirmation email
+2. how can I prove that I am a member of the University? How can I get the discount?
+3. when I booked a facility, the time is not right:the start time is 4pm and the end time is 9am.And I can book the day before today, like 9th May. It is not logic.
+4. I could not see what exact time I have booked(there is just the end time).
+5. (confuse) I just wonder that is it right that I can see other members booking on this calendar as an user.
+6. as an user, I can cancel other member's booking? That is not right.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>7. the 3) 4) I have not tested, I want to test it after the booking part is finished.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>well done.
+I will test it again after the booking part is finished.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -397,6 +456,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -556,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -572,19 +636,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -596,9 +648,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -617,12 +666,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -630,6 +673,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -639,29 +721,14 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1160,182 +1227,182 @@
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="63.83203125" customWidth="1"/>
     <col min="4" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="55.83203125" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:16" ht="29">
+      <c r="A1" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="31"/>
-      <c r="E1" s="26" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="37"/>
+      <c r="E1" s="19" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="40" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:16" ht="40">
+      <c r="A2" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="24" t="s">
+      <c r="J2" s="33"/>
+      <c r="K2" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="20" t="s">
+      <c r="L2" s="33"/>
+      <c r="M2" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="80" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:16" ht="80">
+      <c r="A3" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="22">
+      <c r="D3" s="12"/>
+      <c r="E3" s="17">
         <v>1</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="27" t="s">
+      <c r="J3" s="17"/>
+      <c r="K3" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-    </row>
-    <row r="4" spans="1:16" ht="85" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+    </row>
+    <row r="4" spans="1:16" ht="85">
+      <c r="A4" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="28">
+      <c r="D4" s="12"/>
+      <c r="E4" s="21">
         <v>2</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-    </row>
-    <row r="5" spans="1:16" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+    </row>
+    <row r="5" spans="1:16" ht="68">
+      <c r="A5" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-    </row>
-    <row r="6" spans="1:16" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+    </row>
+    <row r="6" spans="1:16" ht="68">
+      <c r="A6" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:16" ht="29">
+      <c r="A9" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:16" ht="90" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="90">
       <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
@@ -1348,265 +1415,300 @@
       <c r="D10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7" t="s">
+      <c r="F10" s="34"/>
+      <c r="G10" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="34"/>
       <c r="I10" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8" t="s">
+    <row r="11" spans="1:16" s="3" customFormat="1" ht="24">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:16" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:16" s="3" customFormat="1" ht="24">
+      <c r="A12" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-    </row>
-    <row r="13" spans="1:16" ht="136" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+    </row>
+    <row r="13" spans="1:16" ht="306">
+      <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="I13" s="12" t="s">
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:16" ht="40" customHeight="1">
+      <c r="A14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="153" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:16" ht="153">
+      <c r="A15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="11" t="s">
         <v>65</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="187" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:16" ht="187">
+      <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:9" ht="24">
+      <c r="A17" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:9" ht="68">
+      <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="11" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="E18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+    <row r="19" spans="1:9" ht="85">
+      <c r="A19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="I19" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="50" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+    <row r="20" spans="1:9" ht="50">
+      <c r="A20" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="I20" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="119" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:9" ht="119">
+      <c r="A21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="12" t="s">
+      <c r="I21" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:9" ht="24">
+      <c r="A22" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="1:9" ht="187" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:9" ht="272">
+      <c r="A23" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="10" t="s">
         <v>68</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I23" s="12" t="s">
+      <c r="E23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
+    <row r="24" spans="1:9" ht="51">
+      <c r="A24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I24" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="50" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
+    <row r="25" spans="1:9" ht="50">
+      <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="11" t="s">
         <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I25" s="12" t="s">
+      <c r="I25" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="24" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+    <row r="26" spans="1:9" ht="24">
+      <c r="A26" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="1:9" ht="50" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:9" ht="50">
+      <c r="A27" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I27" s="12" t="s">
+      <c r="E27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I27" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
+    <row r="28" spans="1:9" ht="102">
+      <c r="A28" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I28" s="12" t="s">
+      <c r="I28" s="8" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A12:C12"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A12:C12"/>
   </mergeCells>
-  <conditionalFormatting sqref="G10:H10 A10:E10 A13:H16 D11:H12 A12 A18:H21 A17 D17:H17 A23:H25 A22 D22:H22 A27:H28 A26 D26:H26 A3:D4 A5:H8">
+  <conditionalFormatting sqref="G10:H10 A10:E10 D11:H12 A12 A18:H21 A17 D17:H17 A23:H25 A22 D22:H22 A27:H28 A26 D26:H26 A3:D4 A5:H8 A13:H16">
     <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="S4">
       <formula>NOT(ISERROR(SEARCH("S4",A3)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
add a test feedback for email function
</commit_message>
<xml_diff>
--- a/test/Test.xlsx
+++ b/test/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/DUS/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DB3247-7D0C-B04A-A94B-47D3D224E3EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31941E5-06A3-B542-8C0C-ADEF25B59E4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28420" windowHeight="17040" xr2:uid="{2CF56C27-F1AE-2F4B-AFC0-F9C85D1AAA72}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -385,6 +385,25 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>3.1 I can submit the register even if I didn't give the comfirmation code.(there is just alert box once)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 4.the password should be inputted twice for double check.
 5.the password should be 6-20 length.
 6.the password should only contain letters and numbers, but when I input  this:"," it also could work.
@@ -392,6 +411,9 @@
 7.1 "ID", this word, may make confuse to users, it can be changed to "username"
 7.2 "name" may be divided into "first name" and "last name". That will be better I think.</t>
     </r>
+  </si>
+  <si>
+    <t>3,1</t>
   </si>
 </sst>
 </file>
@@ -642,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -722,6 +744,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -734,24 +771,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -942,15 +965,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>2222500</xdr:rowOff>
+      <xdr:rowOff>1968500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4025900</xdr:colOff>
+      <xdr:colOff>4013200</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>3314700</xdr:rowOff>
+      <xdr:rowOff>3060700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -973,8 +996,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12471400" y="9448800"/>
+          <a:off x="12458700" y="9194800"/>
           <a:ext cx="4000500" cy="1092200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>760877</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F2584F9-56C7-434A-9FE5-C6F43D5BC78A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22301200" y="6769100"/>
+          <a:ext cx="7797800" cy="8926977"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1297,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5101827C-6188-DB4F-BA72-CCBBDACC9237}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1313,11 +1380,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
       <c r="E1" s="19" t="s">
         <v>71</v>
       </c>
@@ -1344,14 +1411,14 @@
       <c r="H2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="I2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="40"/>
-      <c r="K2" s="39" t="s">
+      <c r="J2" s="34"/>
+      <c r="K2" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="40"/>
+      <c r="L2" s="34"/>
       <c r="M2" s="15" t="s">
         <v>41</v>
       </c>
@@ -1460,17 +1527,17 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="29">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:16" ht="90">
@@ -1496,6 +1563,9 @@
       <c r="H10" s="35"/>
       <c r="I10" s="5" t="s">
         <v>41</v>
+      </c>
+      <c r="N10" s="41" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="3" customFormat="1" ht="24">
@@ -1518,11 +1588,11 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" ht="24">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
     </row>
     <row r="13" spans="1:16" ht="409.6">
       <c r="A13" s="8" t="s">
@@ -1599,11 +1669,11 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="24">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:9" ht="68">
@@ -1669,11 +1739,11 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="24">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
       <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9" ht="272">
@@ -1725,11 +1795,11 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="24">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
       <c r="I26" s="8"/>
     </row>
     <row r="27" spans="1:9" ht="50">
@@ -1768,16 +1838,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A17:C17"/>
   </mergeCells>
   <conditionalFormatting sqref="G10:H10 A10:E10 D11:H12 A12 A18:H21 A17 D17:H17 A23:H25 A22 D22:H22 A27:H28 A26 D26:H26 A3:D4 A5:H8 A13:H16">
     <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="S4">

</xml_diff>

<commit_message>
new test for user part(just a minor detail)
</commit_message>
<xml_diff>
--- a/test/Test.xlsx
+++ b/test/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/DUS/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56B6E53-39ED-5943-A13E-BE9F95F872D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF6ABB7-285D-6942-BE27-6EBFB4CD9798}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
   <si>
     <t>ID</t>
   </si>
@@ -625,6 +625,38 @@
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
+    <t>well done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">well done.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">S3
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1.just want to make sure: does the user have the right to delete himself  account?
+2.suggestion is same with the right-&gt;</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">S2
 1. </t>
@@ -675,7 +707,6 @@
     </r>
     <r>
       <rPr>
-        <strike/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri (Body)"/>
@@ -693,16 +724,6 @@
       <t xml:space="preserve">
 7.2 "name" may be divided into "first name" and "last name". That will be better I think.</t>
     </r>
-  </si>
-  <si>
-    <t>well done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">well done.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <r>
@@ -768,12 +789,22 @@
         <color theme="1"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>7. suggestion:
+      <t xml:space="preserve">7. suggestion:
 7.1 the page can show that how many the left capacity is of the facility so that the user will not be confused when the capacity is met and they cannot book it.
-7.2 I don't know what exactly others book on the calendar when the facility is "all" . &lt;&lt;&lt;&lt;&lt;&lt;------like the screenshot on the left</t>
-    </r>
-    <r>
-      <rPr>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>7.2 I don't know what exactly others book on the calendar when the facility is "all" . &lt;&lt;&lt;&lt;&lt;&lt;------like the screenshot on the left</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -785,6 +816,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
@@ -793,33 +825,15 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">S3
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>1.just want to make sure: does the user have the right to delete himself  account?
-2.suggestion is same with the right-&gt;</t>
-    </r>
+    <t>S2
+As an user, he can add facility in the home page? That's not right</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -966,6 +980,20 @@
       <sz val="12"/>
       <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1232,6 +1260,27 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1243,27 +1292,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1615,50 +1643,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>44484</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>4058</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1743934</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>296333</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32A0D197-1865-5C4B-A94C-401F201DB5F1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10529040" y="21368280"/>
-          <a:ext cx="1699450" cy="4920720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1717,7 +1701,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1769,7 +1753,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1973,8 +1957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1989,11 +1973,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="42"/>
       <c r="E1" s="19" t="s">
         <v>61</v>
       </c>
@@ -2020,14 +2004,14 @@
       <c r="H2" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="41" t="s">
+      <c r="J2" s="49"/>
+      <c r="K2" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="42"/>
+      <c r="L2" s="49"/>
       <c r="M2" s="15" t="s">
         <v>34</v>
       </c>
@@ -2136,17 +2120,17 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="29">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:16" ht="90">
@@ -2162,14 +2146,14 @@
       <c r="D10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43" t="s">
+      <c r="F10" s="44"/>
+      <c r="G10" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="43"/>
+      <c r="H10" s="44"/>
       <c r="I10" s="5" t="s">
         <v>34</v>
       </c>
@@ -2195,11 +2179,11 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" ht="24">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
     </row>
     <row r="13" spans="1:16" ht="289">
       <c r="A13" s="8" t="s">
@@ -2218,7 +2202,7 @@
         <v>68</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H13" s="33" t="s">
         <v>70</v>
@@ -2244,7 +2228,7 @@
         <v>68</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H14" t="s">
         <v>69</v>
@@ -2292,8 +2276,8 @@
       <c r="F16" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="49" t="s">
-        <v>96</v>
+      <c r="G16" s="39" t="s">
+        <v>94</v>
       </c>
       <c r="H16" s="33" t="s">
         <v>84</v>
@@ -2303,11 +2287,11 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="24">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:9" ht="68">
@@ -2346,8 +2330,14 @@
       <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
       <c r="F19" t="s">
         <v>71</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="H19" s="36" t="s">
         <v>78</v>
@@ -2397,11 +2387,11 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="24">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
       <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9" ht="340">
@@ -2418,7 +2408,7 @@
         <v>64</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>38</v>
@@ -2438,7 +2428,7 @@
         <v>71</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H24" s="37" t="s">
         <v>69</v>
@@ -2468,11 +2458,11 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="24">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
       <c r="I26" s="8"/>
     </row>
     <row r="27" spans="1:9" ht="50">
@@ -2489,7 +2479,7 @@
         <v>64</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>38</v>
@@ -2517,16 +2507,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A9:I9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="G10:H10 A10:E10 D11:H12 A12 A18:H21 A17 D17:H17 A23:H25 A22 D22:H22 A27:H28 A26 D26:H26 A3:D4 A5:H8 A13:H16">

</xml_diff>

<commit_message>
Test report and presentation slides updated
</commit_message>
<xml_diff>
--- a/test/Test.xlsx
+++ b/test/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/DUS/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA69D74-A728-554B-BDD8-DA04E1C55AE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBDA0EC-206E-DB43-8BC0-BC93AB2DAF6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="1320" windowWidth="26000" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2800" yWindow="480" windowWidth="26000" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -562,10 +562,6 @@
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>Bug Classification</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
     <t>FR2.x Facility Related Functional Requirements</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
@@ -905,6 +901,9 @@
   </si>
   <si>
     <t>Why remove the css?</t>
+  </si>
+  <si>
+    <t>Bug Classification</t>
   </si>
 </sst>
 </file>
@@ -1330,6 +1329,21 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1342,23 +1356,8 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1812,7 +1811,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1864,7 +1863,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2068,15 +2067,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="63.83203125" customWidth="1"/>
+    <col min="3" max="3" width="53.83203125" customWidth="1"/>
     <col min="4" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
     <col min="7" max="7" width="55.83203125" customWidth="1"/>
@@ -2084,11 +2083,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29">
-      <c r="A1" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="41"/>
+      <c r="A1" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
       <c r="E1" s="19" t="s">
         <v>61</v>
       </c>
@@ -2115,19 +2114,19 @@
       <c r="H2" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="48"/>
-      <c r="K2" s="47" t="s">
+      <c r="J2" s="42"/>
+      <c r="K2" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="48"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="60">
+    <row r="3" spans="1:16" ht="76" customHeight="1">
       <c r="A3" s="22" t="s">
         <v>48</v>
       </c>
@@ -2195,7 +2194,7 @@
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
     </row>
-    <row r="5" spans="1:16" ht="68">
+    <row r="5" spans="1:16" ht="83" customHeight="1">
       <c r="A5" s="22" t="s">
         <v>54</v>
       </c>
@@ -2231,17 +2230,17 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="29">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:16" ht="90">
@@ -2290,11 +2289,11 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" ht="24">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
     </row>
     <row r="13" spans="1:16" ht="409.6">
       <c r="A13" s="8" t="s">
@@ -2313,7 +2312,7 @@
         <v>67</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H13" s="33" t="s">
         <v>70</v>
@@ -2365,7 +2364,7 @@
         <v>67</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H15" s="34" t="s">
         <v>75</v>
@@ -2391,7 +2390,7 @@
         <v>67</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H16" s="33" t="s">
         <v>84</v>
@@ -2401,11 +2400,11 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="24">
-      <c r="A17" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
+      <c r="A17" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:9" ht="68">
@@ -2413,10 +2412,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -2495,11 +2494,11 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="24">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
       <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9" ht="255">
@@ -2516,7 +2515,7 @@
         <v>64</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>38</v>
@@ -2563,11 +2562,11 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="24">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
       <c r="I26" s="8"/>
     </row>
     <row r="27" spans="1:9" ht="50">
@@ -2584,7 +2583,7 @@
         <v>64</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>38</v>
@@ -2595,7 +2594,7 @@
         <v>32</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>33</v>
@@ -2604,7 +2603,7 @@
         <v>71</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>36</v>
@@ -2612,21 +2611,21 @@
     </row>
     <row r="29" spans="1:9" ht="97" customHeight="1">
       <c r="G29" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A17:C17"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="G10:H10 A10:E10 D11:H12 A12 A18:H21 A17 D17:H17 A23:H25 A22 D22:H22 A27:H28 A26 D26:H26 A3:D4 A5:H8 A13:H16">
@@ -2699,7 +2698,7 @@
       <formula>NOT(ISERROR(SEARCH("S1",H16)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$B$3:$B$6</formula1>
     </dataValidation>

</xml_diff>